<commit_message>
Fix IP bug in accounting
</commit_message>
<xml_diff>
--- a/LTCM's Revenge V2/SpartanTrader/SpartanTrader.xlsx
+++ b/LTCM's Revenge V2/SpartanTrader/SpartanTrader.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stf2jh.MCINTIRE\Desktop\My Safe Space\LTCM's Revenge\SpartanTrader\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stf2jh\Desktop\My Safe Space\LTCM's Revenge V2\SpartanTrader\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22530" windowHeight="8865" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18930" windowHeight="7845"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,12 @@
     <definedName name="APCell">Dashboard!$F$11</definedName>
     <definedName name="CAccountATCell">Dashboard!$C$15</definedName>
     <definedName name="CAccountCell">Dashboard!$F$4</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"d61e4b85-7e3f-4d53-b204-d6a30234d16b"</definedName>
     <definedName name="CurrentDateCell">Dashboard!$B$1</definedName>
     <definedName name="DeltaCell">Dashboard!$C$9</definedName>
+    <definedName name="DeltaGammaRatioRange">Dashboard!$P$4:$P$15</definedName>
     <definedName name="FamilyDeltaRange">Dashboard!$J$4:$J$15</definedName>
+    <definedName name="FamilyGammaRange">Dashboard!$O$4:$O$15</definedName>
     <definedName name="InterestSLT">Dashboard!#REF!</definedName>
     <definedName name="InterestSLTCell">Dashboard!$C$16</definedName>
     <definedName name="IPCell">Dashboard!$F$10</definedName>
@@ -63,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
   <si>
     <t>Column1</t>
   </si>
@@ -214,6 +217,12 @@
   <si>
     <t>Team 16</t>
   </si>
+  <si>
+    <t>FamGam</t>
+  </si>
+  <si>
+    <t>Delta/Gamma Ratio</t>
+  </si>
 </sst>
 </file>
 
@@ -228,7 +237,7 @@
     <numFmt numFmtId="166" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +318,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -348,7 +363,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -374,6 +389,15 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -381,7 +405,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -426,6 +450,8 @@
     <xf numFmtId="9" fontId="11" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="6" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -444,7 +470,7 @@
     <xf numFmtId="43" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -453,9 +479,6 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="36">
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -503,6 +526,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -700,17 +726,17 @@
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.TextBox"/>
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1E12A053B1DE601403C1929712C49806526431"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="3444E796F32E5634DBB3AD443DA96C96AFE363"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="5821"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="688"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -720,14 +746,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="79D0D609B7DFF37480F7BB527498A95790DFE7"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2311F09D4218142487C2A3502B61EAD69D6562"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1905"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -737,14 +763,14 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="6CDE2141D694EB644F46B4D964364FAB57F7D6"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="265EE0AA020FCB24ED32A2E6289C23A4A284A2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="2672"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="661"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -754,31 +780,31 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="58BD0BD1D56EA9547CB5B11250BD777D38F3C5"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1146D4AA719FCE14CB2183A814563A0114F691"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="2540"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
 <file path=xl/activeX/activeX13.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.TextBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="4804B894B4625B44B2A48BD24D6E1289DAA604"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="14D2E6EA61825D1412118B6A10DC5CB8551F61"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1905"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="11377"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="3440"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -802,17 +828,17 @@
 
 <file path=xl/activeX/activeX15.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.TextBox"/>
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="14D2E6EA61825D1412118B6A10DC5CB8551F61"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="4804B894B4625B44B2A48BD24D6E1289DAA604"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="11377"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="3440"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1905"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -822,7 +848,75 @@
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1146D4AA719FCE14CB2183A814563A0114F691"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="58BD0BD1D56EA9547CB5B11250BD777D38F3C5"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="2540"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX17.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="6CDE2141D694EB644F46B4D964364FAB57F7D6"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="2672"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="661"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX18.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="79D0D609B7DFF37480F7BB527498A95790DFE7"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1905"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX19.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="80BBA96708804184A0489ACF8A7FDAB7160D68"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="9816"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="953"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="24591057C2A904240DD28D3C223812D8CA7DB2"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -834,58 +928,109 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX20.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="265EE0AA020FCB24ED32A2E6289C23A4A284A2"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="9D830DCB29BC029417298B929A478EA3C0FA69"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3651"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="741"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX21.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2311F09D4218142487C2A3502B61EAD69D6562"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="18A41690311C3F141861BEF41E0BB7842FCC71"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1905"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX22.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="222A5BEB82BE7824A612A77228E43D1409B532"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1BE1EB35E15CDC14C2218A9D1015FBA9B602A1"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="2540"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX23.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1CA51F704169A314A841A72C1CBB6845AA7AE1"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="2672"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="661"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX24.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="196049FDA184AE147CE1BBE81E5C0044DD3AB1"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1905"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX25.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1A5300D1519D8614C651A5E41EA58707E32A91"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="9843"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="953"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX26.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.TextBox"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -902,7 +1047,143 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX27.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.TextBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1E12A053B1DE601403C1929712C49806526431"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="5821"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="688"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX28.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ListBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2F75D80EE24C9C248F42BF97298610941F8052"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3175"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="9631"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX29.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ListBox"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="1421938551B91514FF419CCD1E8FECE2FBDC71"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="3175"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="9102"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="268F662502FE1624A94299F620E8E0A471D302"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2234A56B92A13D244042A8A42709A6270F30E2"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="24F8E3D6B28DE5245CE296E7221D05A1AA2B22"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2E33B010025BDE242412937C21D1E8099047A2"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX7.xml><?xml version="1.0" encoding="utf-8"?>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
+  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
+  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
+  <ax:ocxPr ax:name="Cookie" ax:value="2BD16582D2BDCF2477F288692C47090B6E7902"/>
+  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
+  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
+  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
+  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
+  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
+  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
+</ax:ocx>
+</file>
+
+<file path=xl/activeX/activeX8.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
@@ -919,12 +1200,12 @@
 </ax:ocx>
 </file>
 
-<file path=xl/activeX/activeX21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/activeX/activeX9.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
   <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
   <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
   <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2BD16582D2BDCF2477F288692C47090B6E7902"/>
+  <ax:ocxPr ax:name="Cookie" ax:value="222A5BEB82BE7824A612A77228E43D1409B532"/>
   <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
   <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
@@ -932,261 +1213,6 @@
   <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
   <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
   <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX22.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2E33B010025BDE242412937C21D1E8099047A2"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX23.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="24F8E3D6B28DE5245CE296E7221D05A1AA2B22"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX24.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2234A56B92A13D244042A8A42709A6270F30E2"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX25.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="268F662502FE1624A94299F620E8E0A471D302"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX26.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="24591057C2A904240DD28D3C223812D8CA7DB2"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX27.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="3444E796F32E5634DBB3AD443DA96C96AFE363"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1349"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="265"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX28.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ListBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1421938551B91514FF419CCD1E8FECE2FBDC71"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3175"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="9102"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX29.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ListBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="2F75D80EE24C9C248F42BF97298610941F8052"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3175"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="9631"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX3.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1A5300D1519D8614C651A5E41EA58707E32A91"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="9843"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="953"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="196049FDA184AE147CE1BBE81E5C0044DD3AB1"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1905"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1CA51F704169A314A841A72C1CBB6845AA7AE1"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="2672"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="661"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX6.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="1BE1EB35E15CDC14C2218A9D1015FBA9B602A1"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="2540"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX7.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="18A41690311C3F141861BEF41E0BB7842FCC71"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="1905"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="714"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX8.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.ComboBox"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="9D830DCB29BC029417298B929A478EA3C0FA69"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="3651"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="741"/>
-  <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
-</ax:ocx>
-</file>
-
-<file path=xl/activeX/activeX9.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{A37BBB42-E8C1-4E09-B9CA-F009CE620C08}" ax:persistence="persistPropertyBag">
-  <ax:ocxPr ax:name="RawObjectTypeName" ax:value="System.Windows.Forms.Button"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyName" ax:value="System.Windows.Forms, Version=4.0.0.0, Culture=neutral, PublicKeyToken=b77a5c561934e089"/>
-  <ax:ocxPr ax:name="RawObjectAssemblyPath" ax:value=""/>
-  <ax:ocxPr ax:name="Cookie" ax:value="80BBA96708804184A0489ACF8A7FDAB7160D68"/>
-  <ax:ocxPr ax:name="ControlInfo_cb" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_hAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_cAccel" ax:value="0"/>
-  <ax:ocxPr ax:name="ControlInfo_dwFlags" ax:value="0"/>
-  <ax:ocxPr ax:name="MiscStatusBits" ax:value="0"/>
-  <ax:ocxPr ax:name="Sizel_cx" ax:value="9816"/>
-  <ax:ocxPr ax:name="Sizel_cy" ax:value="953"/>
   <ax:ocxPr ax:name="IsDynamic" ax:value="0"/>
 </ax:ocx>
 </file>
@@ -1368,11 +1394,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="490793040"/>
-        <c:axId val="490793432"/>
+        <c:axId val="448789160"/>
+        <c:axId val="448789552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="490793040"/>
+        <c:axId val="448789160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1416,7 +1442,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="490793432"/>
+        <c:crossAx val="448789552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1424,7 +1450,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="490793432"/>
+        <c:axId val="448789552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1488,7 +1514,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="490793040"/>
+        <c:crossAx val="448789160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1743,11 +1769,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="492055416"/>
-        <c:axId val="492055808"/>
+        <c:axId val="449477504"/>
+        <c:axId val="449477896"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="492055416"/>
+        <c:axId val="449477504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1789,7 +1815,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492055808"/>
+        <c:crossAx val="449477896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1797,7 +1823,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="492055808"/>
+        <c:axId val="449477896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1848,7 +1874,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492055416"/>
+        <c:crossAx val="449477504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2098,11 +2124,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="492056592"/>
-        <c:axId val="492056984"/>
+        <c:axId val="449478680"/>
+        <c:axId val="449479072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="492056592"/>
+        <c:axId val="449478680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2144,7 +2170,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492056984"/>
+        <c:crossAx val="449479072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2152,7 +2178,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="492056984"/>
+        <c:axId val="449479072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2203,7 +2229,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="492056592"/>
+        <c:crossAx val="449478680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5763,11 +5789,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="TransactionQueueLO" displayName="TransactionQueueLO" ref="B2:G14" totalsRowShown="0" headerRowCellStyle="Comma" dataCellStyle="Comma">
   <autoFilter ref="B2:G14"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Column1" dataDxfId="5" dataCellStyle="Comma"/>
-    <tableColumn id="2" name="Column2" dataDxfId="4" dataCellStyle="Comma"/>
-    <tableColumn id="3" name="Column3" dataDxfId="3" dataCellStyle="Comma"/>
-    <tableColumn id="4" name="Column4" dataDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="5" name="Column5" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="1" name="Column1" dataDxfId="4" dataCellStyle="Comma"/>
+    <tableColumn id="2" name="Column2" dataDxfId="3" dataCellStyle="Comma"/>
+    <tableColumn id="3" name="Column3" dataDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="4" name="Column4" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="5" name="Column5" dataDxfId="0" dataCellStyle="Comma"/>
     <tableColumn id="6" name="Column6" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5844,7 +5870,7 @@
     <tableColumn id="2" name="Column2" dataCellStyle="Comma"/>
     <tableColumn id="3" name="Column3" dataCellStyle="Comma"/>
     <tableColumn id="4" name="Column4" dataCellStyle="Comma"/>
-    <tableColumn id="5" name="Column5" dataDxfId="0" dataCellStyle="Comma"/>
+    <tableColumn id="5" name="Column5" dataDxfId="16" dataCellStyle="Comma"/>
     <tableColumn id="6" name="Column6" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5852,28 +5878,28 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="OptionMarketLO" displayName="OptionMarketLO" ref="I2:P8" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" headerRowCellStyle="Comma" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="OptionMarketLO" displayName="OptionMarketLO" ref="I2:P8" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" headerRowCellStyle="Comma" dataCellStyle="Comma">
   <autoFilter ref="I2:P8"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Column1" dataDxfId="14" dataCellStyle="Comma"/>
-    <tableColumn id="2" name="Column2" dataDxfId="13" dataCellStyle="Comma"/>
+    <tableColumn id="1" name="Column1" dataDxfId="13" dataCellStyle="Comma"/>
+    <tableColumn id="2" name="Column2" dataDxfId="12" dataCellStyle="Comma"/>
     <tableColumn id="3" name="Column3" dataCellStyle="Comma"/>
     <tableColumn id="4" name="Column4" dataCellStyle="Comma"/>
     <tableColumn id="5" name="Column5" dataCellStyle="Comma"/>
-    <tableColumn id="6" name="Column6" dataDxfId="12" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="Column7" dataDxfId="11" dataCellStyle="Comma"/>
-    <tableColumn id="8" name="Column8" dataDxfId="10" dataCellStyle="Comma"/>
+    <tableColumn id="6" name="Column6" dataDxfId="11" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="Column7" dataDxfId="10" dataCellStyle="Comma"/>
+    <tableColumn id="8" name="Column8" dataDxfId="9" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="SP500LO" displayName="SP500LO" ref="R2:T8" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8" headerRowCellStyle="Comma" dataCellStyle="Comma">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="SP500LO" displayName="SP500LO" ref="R2:T8" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowCellStyle="Comma" dataCellStyle="Comma">
   <autoFilter ref="R2:T8"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Column1" dataDxfId="7" dataCellStyle="Comma"/>
-    <tableColumn id="2" name="Column2" dataDxfId="6" dataCellStyle="Comma"/>
+    <tableColumn id="1" name="Column1" dataDxfId="6" dataCellStyle="Comma"/>
+    <tableColumn id="2" name="Column2" dataDxfId="5" dataCellStyle="Comma"/>
     <tableColumn id="3" name="Column3" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6169,8 +6195,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:AD50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4:P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6188,24 +6214,24 @@
     <col min="11" max="11" width="12.5703125" style="7" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" style="7" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="7"/>
-    <col min="14" max="14" width="10.5703125" style="7" customWidth="1"/>
-    <col min="15" max="26" width="9.140625" style="7"/>
+    <col min="14" max="15" width="10.5703125" style="7" customWidth="1"/>
+    <col min="16" max="26" width="9.140625" style="7"/>
     <col min="27" max="30" width="11.140625" style="7" customWidth="1"/>
     <col min="31" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:30" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="O1" s="37" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="O1" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
     </row>
     <row r="2" spans="2:30" ht="21" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="13" t="s">
@@ -6233,6 +6259,12 @@
       </c>
       <c r="M2" s="32" t="s">
         <v>48</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="37" t="s">
+        <v>51</v>
       </c>
       <c r="AA2" s="7" t="s">
         <v>0</v>
@@ -6275,6 +6307,12 @@
       <c r="K4" s="34"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
+      <c r="O4" s="44">
+        <v>0</v>
+      </c>
+      <c r="P4" s="44">
+        <v>0</v>
+      </c>
       <c r="AA4" s="6"/>
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
@@ -6299,6 +6337,12 @@
       <c r="K5" s="34"/>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
+      <c r="O5" s="44">
+        <v>0</v>
+      </c>
+      <c r="P5" s="44">
+        <v>0</v>
+      </c>
       <c r="AA5" s="6"/>
       <c r="AB5" s="6"/>
       <c r="AC5" s="6"/>
@@ -6321,6 +6365,12 @@
       <c r="K6" s="34"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
+      <c r="O6" s="44">
+        <v>0</v>
+      </c>
+      <c r="P6" s="44">
+        <v>0</v>
+      </c>
       <c r="AA6" s="6"/>
       <c r="AB6" s="6"/>
       <c r="AC6" s="6"/>
@@ -6339,6 +6389,12 @@
       <c r="K7" s="34"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
+      <c r="O7" s="44">
+        <v>0</v>
+      </c>
+      <c r="P7" s="44">
+        <v>0</v>
+      </c>
       <c r="AA7" s="6"/>
       <c r="AB7" s="6"/>
       <c r="AC7" s="6"/>
@@ -6359,6 +6415,12 @@
       <c r="K8" s="34"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
+      <c r="O8" s="44">
+        <v>0</v>
+      </c>
+      <c r="P8" s="44">
+        <v>0</v>
+      </c>
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
       <c r="AC8" s="6"/>
@@ -6377,6 +6439,12 @@
       <c r="K9" s="34"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
+      <c r="O9" s="44">
+        <v>0</v>
+      </c>
+      <c r="P9" s="44">
+        <v>0</v>
+      </c>
       <c r="AA9" s="6"/>
       <c r="AB9" s="6"/>
       <c r="AC9" s="6"/>
@@ -6395,6 +6463,12 @@
       <c r="K10" s="34"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
+      <c r="O10" s="44">
+        <v>0</v>
+      </c>
+      <c r="P10" s="44">
+        <v>0</v>
+      </c>
       <c r="AA10" s="6"/>
       <c r="AB10" s="6"/>
       <c r="AC10" s="6"/>
@@ -6419,6 +6493,12 @@
       <c r="K11" s="34"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
+      <c r="O11" s="44">
+        <v>0</v>
+      </c>
+      <c r="P11" s="44">
+        <v>0</v>
+      </c>
       <c r="AA11" s="6"/>
       <c r="AB11" s="6"/>
       <c r="AC11" s="6"/>
@@ -6439,6 +6519,12 @@
       <c r="K12" s="34"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
+      <c r="O12" s="44">
+        <v>0</v>
+      </c>
+      <c r="P12" s="44">
+        <v>0</v>
+      </c>
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
       <c r="AC12" s="6"/>
@@ -6463,6 +6549,12 @@
       <c r="K13" s="34"/>
       <c r="L13" s="6"/>
       <c r="M13" s="6"/>
+      <c r="O13" s="44">
+        <v>0</v>
+      </c>
+      <c r="P13" s="44">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B14" s="6"/>
@@ -6478,6 +6570,12 @@
       <c r="K14" s="34"/>
       <c r="L14" s="6"/>
       <c r="M14" s="6"/>
+      <c r="O14" s="44">
+        <v>0</v>
+      </c>
+      <c r="P14" s="44">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
@@ -6498,6 +6596,12 @@
       <c r="K15" s="34"/>
       <c r="L15" s="6"/>
       <c r="M15" s="6"/>
+      <c r="O15" s="44">
+        <v>0</v>
+      </c>
+      <c r="P15" s="44">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:30" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
@@ -6553,7 +6657,7 @@
       <c r="C24" s="15"/>
       <c r="D24" s="15"/>
       <c r="E24" s="15"/>
-      <c r="F24" s="38">
+      <c r="F24" s="40">
         <v>0</v>
       </c>
     </row>
@@ -6562,22 +6666,22 @@
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
-      <c r="F25" s="38"/>
+      <c r="F25" s="40"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="38"/>
+      <c r="F26" s="40"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="38"/>
+      <c r="F27" s="40"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="38"/>
+      <c r="F28" s="40"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="38"/>
+      <c r="F29" s="40"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F30" s="38"/>
+      <c r="F30" s="40"/>
     </row>
     <row r="39" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="10"/>
@@ -6632,8 +6736,658 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1041" r:id="rId4" name="_ActiveXWrapper2">
+        <control shapeId="1054" r:id="rId4" name="_ActiveXWrapper27">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>600075</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1054" r:id="rId4" name="_ActiveXWrapper27"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1053" r:id="rId6" name="_ActiveXWrapper26">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>600075</xdr:colOff>
+                <xdr:row>13</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1053" r:id="rId6" name="_ActiveXWrapper26"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1052" r:id="rId7" name="_ActiveXWrapper25">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>600075</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1052" r:id="rId7" name="_ActiveXWrapper25"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1051" r:id="rId8" name="_ActiveXWrapper24">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>600075</xdr:colOff>
+                <xdr:row>11</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1051" r:id="rId8" name="_ActiveXWrapper24"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1050" r:id="rId9" name="_ActiveXWrapper23">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>600075</xdr:colOff>
+                <xdr:row>10</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1050" r:id="rId9" name="_ActiveXWrapper23"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1049" r:id="rId10" name="_ActiveXWrapper22">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>600075</xdr:colOff>
+                <xdr:row>9</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1049" r:id="rId10" name="_ActiveXWrapper22"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1048" r:id="rId11" name="_ActiveXWrapper21">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>600075</xdr:colOff>
+                <xdr:row>8</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1048" r:id="rId11" name="_ActiveXWrapper21"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1047" r:id="rId12" name="_ActiveXWrapper20">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>600075</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1047" r:id="rId12" name="_ActiveXWrapper20"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1046" r:id="rId13" name="_ActiveXWrapper19">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>600075</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1046" r:id="rId13" name="_ActiveXWrapper19"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1045" r:id="rId14" name="_ActiveXWrapper18">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>600075</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1045" r:id="rId14" name="_ActiveXWrapper18"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1044" r:id="rId15" name="_ActiveXWrapper17">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>600075</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1044" r:id="rId15" name="_ActiveXWrapper17"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1043" r:id="rId16" name="_ActiveXWrapper16">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>600075</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1043" r:id="rId16" name="_ActiveXWrapper16"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1042" r:id="rId17" name="_ActiveXWrapper32">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>40</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>428625</xdr:colOff>
+                <xdr:row>47</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1042" r:id="rId17" name="_ActiveXWrapper32"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1025" r:id="rId19" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>66675</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>361950</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1025" r:id="rId19" name="_ActiveXWrapper1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1028" r:id="rId21" name="_ActiveXWrapper3">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId22">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>76200</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>762000</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1028" r:id="rId21" name="_ActiveXWrapper3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1029" r:id="rId23" name="_ActiveXWrapper4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId24">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>962025</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1029" r:id="rId23" name="_ActiveXWrapper4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1030" r:id="rId25" name="_ActiveXWrapper5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId26">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>638175</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>561975</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1030" r:id="rId25" name="_ActiveXWrapper5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1031" r:id="rId27" name="_ActiveXWrapper6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId28">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>866775</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>533400</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1031" r:id="rId27" name="_ActiveXWrapper6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1032" r:id="rId29" name="_ActiveXWrapper7">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId30">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>27</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>923925</xdr:colOff>
+                <xdr:row>29</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1032" r:id="rId29" name="_ActiveXWrapper7"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1033" r:id="rId31" name="_ActiveXWrapper8">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>66675</xdr:colOff>
+                <xdr:row>31</xdr:row>
+                <xdr:rowOff>66675</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>361950</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1033" r:id="rId31" name="_ActiveXWrapper8"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1035" r:id="rId33" name="_ActiveXWrapper10">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>85725</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>771525</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1035" r:id="rId33" name="_ActiveXWrapper10"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1036" r:id="rId34" name="_ActiveXWrapper11">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId35">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>933450</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1036" r:id="rId34" name="_ActiveXWrapper11"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1037" r:id="rId36" name="_ActiveXWrapper12">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId26">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>609600</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>133350</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>533400</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1037" r:id="rId36" name="_ActiveXWrapper12"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1038" r:id="rId37" name="_ActiveXWrapper13">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId28">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>847725</xdr:colOff>
+                <xdr:row>33</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>514350</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1038" r:id="rId37" name="_ActiveXWrapper13"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1039" r:id="rId38" name="_ActiveXWrapper14">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId39">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>66675</xdr:colOff>
+                <xdr:row>35</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>942975</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1039" r:id="rId38" name="_ActiveXWrapper14"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1040" r:id="rId40" name="_ActiveXWrapper15">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId41">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>23</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>933450</xdr:colOff>
+                <xdr:row>25</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1040" r:id="rId40" name="_ActiveXWrapper15"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1041" r:id="rId42" name="_ActiveXWrapper2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId43">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>2</xdr:col>
@@ -6652,657 +7406,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1041" r:id="rId4" name="_ActiveXWrapper2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1040" r:id="rId6" name="_ActiveXWrapper15">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>933450</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1040" r:id="rId6" name="_ActiveXWrapper15"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1039" r:id="rId8" name="_ActiveXWrapper14">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>66675</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>942975</xdr:colOff>
-                <xdr:row>38</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1039" r:id="rId8" name="_ActiveXWrapper14"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1038" r:id="rId10" name="_ActiveXWrapper13">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>847725</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>514350</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1038" r:id="rId10" name="_ActiveXWrapper13"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1037" r:id="rId12" name="_ActiveXWrapper12">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>609600</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>133350</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>533400</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1037" r:id="rId12" name="_ActiveXWrapper12"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1036" r:id="rId14" name="_ActiveXWrapper11">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>933450</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1036" r:id="rId14" name="_ActiveXWrapper11"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1035" r:id="rId16" name="_ActiveXWrapper10">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>85725</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>771525</xdr:colOff>
-                <xdr:row>35</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1035" r:id="rId16" name="_ActiveXWrapper10"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1033" r:id="rId18" name="_ActiveXWrapper8">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>66675</xdr:colOff>
-                <xdr:row>31</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>361950</xdr:colOff>
-                <xdr:row>33</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1033" r:id="rId18" name="_ActiveXWrapper8"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1032" r:id="rId20" name="_ActiveXWrapper7">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>923925</xdr:colOff>
-                <xdr:row>29</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1032" r:id="rId20" name="_ActiveXWrapper7"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1031" r:id="rId22" name="_ActiveXWrapper6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>866775</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>533400</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1031" r:id="rId22" name="_ActiveXWrapper6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1030" r:id="rId23" name="_ActiveXWrapper5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>638175</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>561975</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1030" r:id="rId23" name="_ActiveXWrapper5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId24" name="_ActiveXWrapper4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId25">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>962025</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1029" r:id="rId24" name="_ActiveXWrapper4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1028" r:id="rId26" name="_ActiveXWrapper3">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>76200</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>762000</xdr:colOff>
-                <xdr:row>27</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1028" r:id="rId26" name="_ActiveXWrapper3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId27" name="_ActiveXWrapper1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId28">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>66675</xdr:colOff>
-                <xdr:row>23</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>361950</xdr:colOff>
-                <xdr:row>25</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1025" r:id="rId27" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1042" r:id="rId29" name="_ActiveXWrapper32">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId30">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>40</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>428625</xdr:colOff>
-                <xdr:row>47</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1042" r:id="rId29" name="_ActiveXWrapper32"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1043" r:id="rId31" name="_ActiveXWrapper16">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>600075</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1043" r:id="rId31" name="_ActiveXWrapper16"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1044" r:id="rId33" name="_ActiveXWrapper17">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>600075</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1044" r:id="rId33" name="_ActiveXWrapper17"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1045" r:id="rId34" name="_ActiveXWrapper18">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>600075</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1045" r:id="rId34" name="_ActiveXWrapper18"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1046" r:id="rId35" name="_ActiveXWrapper19">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>600075</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1046" r:id="rId35" name="_ActiveXWrapper19"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1047" r:id="rId36" name="_ActiveXWrapper20">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>600075</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1047" r:id="rId36" name="_ActiveXWrapper20"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1048" r:id="rId37" name="_ActiveXWrapper21">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>600075</xdr:colOff>
-                <xdr:row>8</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1048" r:id="rId37" name="_ActiveXWrapper21"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1049" r:id="rId38" name="_ActiveXWrapper22">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>600075</xdr:colOff>
-                <xdr:row>9</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1049" r:id="rId38" name="_ActiveXWrapper22"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1050" r:id="rId39" name="_ActiveXWrapper23">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>600075</xdr:colOff>
-                <xdr:row>10</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1050" r:id="rId39" name="_ActiveXWrapper23"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1051" r:id="rId40" name="_ActiveXWrapper24">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>600075</xdr:colOff>
-                <xdr:row>11</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1051" r:id="rId40" name="_ActiveXWrapper24"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1052" r:id="rId41" name="_ActiveXWrapper25">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>600075</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1052" r:id="rId41" name="_ActiveXWrapper25"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1053" r:id="rId42" name="_ActiveXWrapper26">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>600075</xdr:colOff>
-                <xdr:row>13</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1053" r:id="rId42" name="_ActiveXWrapper26"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1054" r:id="rId43" name="_ActiveXWrapper27">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId32">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>600075</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1054" r:id="rId43" name="_ActiveXWrapper27"/>
+        <control shapeId="1041" r:id="rId42" name="_ActiveXWrapper2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -7335,18 +7439,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="E1" s="39" t="s">
+      <c r="C1" s="41"/>
+      <c r="E1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="39"/>
-      <c r="H1" s="39" t="s">
+      <c r="F1" s="41"/>
+      <c r="H1" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="39"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="27" t="s">
@@ -7483,7 +7587,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:Y8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -7511,29 +7615,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:25" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="I1" s="40" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="I1" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="R1" s="40" t="s">
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="R1" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
@@ -7598,7 +7702,7 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="42"/>
+      <c r="F3" s="36"/>
       <c r="G3" s="5"/>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
@@ -7617,7 +7721,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="42"/>
+      <c r="F4" s="36"/>
       <c r="G4" s="5"/>
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
@@ -7636,7 +7740,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="42"/>
+      <c r="F5" s="36"/>
       <c r="G5" s="5"/>
       <c r="I5" s="25"/>
       <c r="J5" s="25"/>
@@ -7655,7 +7759,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="42"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="5"/>
       <c r="I6" s="25"/>
       <c r="J6" s="25"/>
@@ -7674,7 +7778,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
-      <c r="F7" s="42"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="5"/>
       <c r="I7" s="25"/>
       <c r="J7" s="25"/>
@@ -7693,7 +7797,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
-      <c r="F8" s="42"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="5"/>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
@@ -7743,15 +7847,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="C1" s="43"/>
+      <c r="E1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
     </row>
     <row r="2" spans="2:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -8011,8 +8115,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="6145" r:id="rId4" name="_ActiveXWrapper1">
+        <control shapeId="6146" r:id="rId4" name="_ActiveXWrapper2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>20</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
+                <xdr:row>38</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="6146" r:id="rId4" name="_ActiveXWrapper2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="6145" r:id="rId6" name="_ActiveXWrapper1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -8031,32 +8160,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="6145" r:id="rId4" name="_ActiveXWrapper1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="6146" r:id="rId6" name="_ActiveXWrapper2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>20</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>152400</xdr:colOff>
-                <xdr:row>38</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="6146" r:id="rId6" name="_ActiveXWrapper2"/>
+        <control shapeId="6145" r:id="rId6" name="_ActiveXWrapper1"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>